<commit_message>
Tidying up the Movement processing notebook
</commit_message>
<xml_diff>
--- a/191015_Deuterium_Transfer_Peak_Areas.xlsx
+++ b/191015_Deuterium_Transfer_Peak_Areas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Documents\Parker_research\GCMS_Stuff\191015\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Documents\Parker_research\DCHC_transfer_Experiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E399A45D-76B8-4281-AE2F-09CB15628ECA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2ABF271-0359-4D09-8D0F-C7BC59D51CE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4340" yWindow="4350" windowWidth="32550" windowHeight="20080" xr2:uid="{0C4FD04D-EEC1-4A1F-94F8-64C84F3860BB}"/>
+    <workbookView xWindow="18420" yWindow="130" windowWidth="19490" windowHeight="19670" xr2:uid="{0C4FD04D-EEC1-4A1F-94F8-64C84F3860BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -466,7 +466,7 @@
   <dimension ref="A1:N52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>